<commit_message>
Rename PS3 Excel Docs
</commit_message>
<xml_diff>
--- a/Problem Sets/ps3/Logs/Excel Documents/SorterC vs SorterF.xlsx
+++ b/Problem Sets/ps3/Logs/Excel Documents/SorterC vs SorterF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenyicui/Library/CloudStorage/OneDrive-Personal/Documents/Education/NUS/Year 1/Semester 2/CS2040S/Problem Sets/ps3/Logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenyicui/Library/CloudStorage/OneDrive-Personal/Documents/Education/NUS/Year 1/Semester 2/CS2040S/CS2040S_ProblemSets/Problem Sets/ps3/Logs/Excel Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB7DD968-E260-FE48-9DAB-01219D70DD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CADB642-BD76-2243-95A0-A20EFD77CCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SorterC vs SorterF" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -24951,15 +24951,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>601133</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25285,11 +25285,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="75" workbookViewId="0">
-      <selection activeCell="U97" sqref="U97"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="75" workbookViewId="0">
+      <selection activeCell="T40" sqref="T40:T63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>